<commit_message>
Hotfix devpo 19460 update battery abbreviations
</commit_message>
<xml_diff>
--- a/import-specification/devices/battery.xlsx
+++ b/import-specification/devices/battery.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="139">
   <si>
     <t>Field Type</t>
   </si>
@@ -143,72 +143,255 @@
     <t>Nominal capacity</t>
   </si>
   <si>
-    <t>B_CHARGE_LEVEL</t>
+    <t>B_E_CHARGE_AC</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>Chargeable Energy</t>
+  </si>
+  <si>
+    <t>B_E_DISCHARGE_AC</t>
+  </si>
+  <si>
+    <t>Dischargeable Energy</t>
+  </si>
+  <si>
+    <t>B_E_EXP</t>
+  </si>
+  <si>
+    <t>Total energy from stacks</t>
+  </si>
+  <si>
+    <t>B_E_EXP_AC</t>
+  </si>
+  <si>
+    <t>Energy export from storage system AC</t>
+  </si>
+  <si>
+    <t>B_E_IMP</t>
+  </si>
+  <si>
+    <t>Total energy to stacks</t>
+  </si>
+  <si>
+    <t>B_E_IMP_AC</t>
+  </si>
+  <si>
+    <t>Energy import to storage system AC</t>
+  </si>
+  <si>
+    <t>B_E_INT_EXP</t>
+  </si>
+  <si>
+    <t>erzeugte Energie pro Intervall (geliefert)</t>
+  </si>
+  <si>
+    <t>B_E_INT_IMP</t>
+  </si>
+  <si>
+    <t>erzeugte Energie pro Intervall (bezogen)</t>
+  </si>
+  <si>
+    <t>B_E_STORED</t>
+  </si>
+  <si>
+    <t>Currently stored energy</t>
+  </si>
+  <si>
+    <t>B_F_AC</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>Grid frequency</t>
+  </si>
+  <si>
+    <t>B_I_AC</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Battery AC current</t>
+  </si>
+  <si>
+    <t>B_I_DC</t>
+  </si>
+  <si>
+    <t>Ladestrom (DC)</t>
+  </si>
+  <si>
+    <t>B_LIM_I_CHARGE</t>
+  </si>
+  <si>
+    <t>B_LIM_I_DISCHARGE</t>
+  </si>
+  <si>
+    <t>B_LIM_P_CHARGE</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Maximum charging power</t>
+  </si>
+  <si>
+    <t>B_LIM_P_DISCHARGE</t>
+  </si>
+  <si>
+    <t>Maximum discharging power</t>
+  </si>
+  <si>
+    <t>B_LIM_U_CHARGE</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Charge end voltage</t>
+  </si>
+  <si>
+    <t>B_LIM_U_DISCHARGE</t>
+  </si>
+  <si>
+    <t>B_OT_TOTAL</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Operating Hours</t>
+  </si>
+  <si>
+    <t>B_P_AC</t>
+  </si>
+  <si>
+    <t>Battery power AC</t>
+  </si>
+  <si>
+    <t>B_P_DC</t>
+  </si>
+  <si>
+    <t>Total battery power</t>
+  </si>
+  <si>
+    <t>B_Q_AC</t>
+  </si>
+  <si>
+    <t>VAr</t>
+  </si>
+  <si>
+    <t>Battery reactive power AC</t>
+  </si>
+  <si>
+    <t>B_SOC</t>
   </si>
   <si>
     <t>%</t>
   </si>
   <si>
-    <t>Charge Level</t>
-  </si>
-  <si>
-    <t>B_E_EXP</t>
-  </si>
-  <si>
-    <t>kWh</t>
-  </si>
-  <si>
-    <t>Total energy from stacks</t>
-  </si>
-  <si>
-    <t>B_E_IMP</t>
-  </si>
-  <si>
-    <t>Total energy to stacks</t>
-  </si>
-  <si>
-    <t>B_E_STORED</t>
-  </si>
-  <si>
-    <t>Currently stored energy</t>
-  </si>
-  <si>
-    <t>B_I_DC</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Ladestrom (DC)</t>
-  </si>
-  <si>
-    <t>B_OT_TOTAL</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>Operating Hours</t>
-  </si>
-  <si>
-    <t>B_P_DC</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>Total battery power</t>
+    <t>State of Charge</t>
+  </si>
+  <si>
+    <t>B_SOCH</t>
+  </si>
+  <si>
+    <t>Ladezustand (Nennkapazität) in %</t>
+  </si>
+  <si>
+    <t>B_SOH</t>
+  </si>
+  <si>
+    <t>Alterungsbedingter Erhaltungszustand in %</t>
+  </si>
+  <si>
+    <t>B_S_AC</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>Battery apparent power AC</t>
+  </si>
+  <si>
+    <t>B_T_CELL[1..x]_[1..x]_[1..x]</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>Cell temperature  [°C]</t>
+  </si>
+  <si>
+    <t>B_T_CELL_MAX[1..x]_[1..x]_[1..x]</t>
+  </si>
+  <si>
+    <t>Maximum cell temperature  [°C]</t>
+  </si>
+  <si>
+    <t>B_T_CELL_MIN[1..x]_[1..x]_[1..x]</t>
+  </si>
+  <si>
+    <t>Minimum cell temperature  [°C]</t>
+  </si>
+  <si>
+    <t>B_T_M[1..x]</t>
+  </si>
+  <si>
+    <t>Module temperature [°C]</t>
+  </si>
+  <si>
+    <t>B_T_M_MAX[1..x]</t>
+  </si>
+  <si>
+    <t>Maximum module temperature [°C]</t>
+  </si>
+  <si>
+    <t>B_T_M_MIN[1..x]</t>
+  </si>
+  <si>
+    <t>Minimum module temperature [°C]</t>
+  </si>
+  <si>
+    <t>B_T_U[1..x]</t>
+  </si>
+  <si>
+    <t>Temperature Outside/ Ambient [°C]</t>
+  </si>
+  <si>
+    <t>B_U_AC</t>
+  </si>
+  <si>
+    <t>Battery AC voltage</t>
   </si>
   <si>
     <t>B_U_BULK</t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
     <t>Battery charging voltage DC</t>
   </si>
   <si>
+    <t>B_U_CELL_AVG</t>
+  </si>
+  <si>
+    <t>Average cell voltage</t>
+  </si>
+  <si>
+    <t>B_U_CELL_MAX[1..x]_[1..x]_[1..x]</t>
+  </si>
+  <si>
+    <t>Maximum cell voltage</t>
+  </si>
+  <si>
+    <t>B_U_CELL_MIN[1..x]_[1..x]_[1..x]</t>
+  </si>
+  <si>
+    <t>Minimum cell voltage</t>
+  </si>
+  <si>
     <t>B_U_DC</t>
   </si>
   <si>
@@ -222,9 +405,6 @@
   </si>
   <si>
     <t>T[1..x]</t>
-  </si>
-  <si>
-    <t>°C</t>
   </si>
   <si>
     <t>Temperatures</t>
@@ -602,7 +782,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -611,7 +791,7 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="17.567139" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="38.847656" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="5.855713" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="54.129639" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="9.283447" bestFit="true" customWidth="true" style="0"/>
@@ -847,10 +1027,10 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
         <v>46</v>
-      </c>
-      <c r="D13" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -858,13 +1038,13 @@
         <v>38</v>
       </c>
       <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
         <v>48</v>
-      </c>
-      <c r="C14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -872,13 +1052,13 @@
         <v>38</v>
       </c>
       <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
         <v>50</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -886,13 +1066,13 @@
         <v>38</v>
       </c>
       <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
         <v>52</v>
-      </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -900,13 +1080,13 @@
         <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -914,13 +1094,13 @@
         <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -928,13 +1108,13 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -942,13 +1122,13 @@
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -956,13 +1136,13 @@
         <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
         <v>62</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -970,13 +1150,13 @@
         <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -984,10 +1164,13 @@
         <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -995,10 +1178,7 @@
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1006,10 +1186,7 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1017,10 +1194,415 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
         <v>77</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D28" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" t="s">
+        <v>121</v>
+      </c>
+      <c r="C48" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" t="s">
+        <v>125</v>
+      </c>
+      <c r="C50" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" t="s">
+        <v>77</v>
+      </c>
+      <c r="D51" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" t="s">
+        <v>101</v>
+      </c>
+      <c r="D52" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" t="s">
+        <v>135</v>
+      </c>
+      <c r="D55" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56" t="s">
+        <v>137</v>
+      </c>
+      <c r="D56" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update battery, ppc import-specification
</commit_message>
<xml_diff>
--- a/import-specification/devices/battery.xlsx
+++ b/import-specification/devices/battery.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="150">
   <si>
     <t>Field Type</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>Charging current DC</t>
+  </si>
+  <si>
+    <t>B_I_DIS_DC</t>
+  </si>
+  <si>
+    <t>Discharging current DC</t>
   </si>
   <si>
     <t>B_LIM_I_CHARGE</t>
@@ -809,7 +815,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1235,6 +1241,9 @@
       <c r="B26" t="s">
         <v>73</v>
       </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
       <c r="D26" t="s">
         <v>74</v>
       </c>
@@ -1257,11 +1266,8 @@
       <c r="B28" t="s">
         <v>77</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>78</v>
-      </c>
-      <c r="D28" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1269,10 +1275,10 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" t="s">
         <v>80</v>
-      </c>
-      <c r="C29" t="s">
-        <v>78</v>
       </c>
       <c r="D29" t="s">
         <v>81</v>
@@ -1286,10 +1292,10 @@
         <v>82</v>
       </c>
       <c r="C30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" t="s">
         <v>83</v>
-      </c>
-      <c r="D30" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1297,6 +1303,9 @@
         <v>38</v>
       </c>
       <c r="B31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" t="s">
         <v>85</v>
       </c>
       <c r="D31" t="s">
@@ -1310,11 +1319,8 @@
       <c r="B32" t="s">
         <v>87</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>88</v>
-      </c>
-      <c r="D32" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1322,10 +1328,10 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
         <v>90</v>
-      </c>
-      <c r="C33" t="s">
-        <v>78</v>
       </c>
       <c r="D33" t="s">
         <v>91</v>
@@ -1339,7 +1345,7 @@
         <v>92</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D34" t="s">
         <v>93</v>
@@ -1353,10 +1359,10 @@
         <v>94</v>
       </c>
       <c r="C35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" t="s">
         <v>95</v>
-      </c>
-      <c r="D35" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1364,13 +1370,13 @@
         <v>38</v>
       </c>
       <c r="B36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" t="s">
         <v>97</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>98</v>
-      </c>
-      <c r="D36" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1378,10 +1384,10 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" t="s">
         <v>100</v>
-      </c>
-      <c r="C37" t="s">
-        <v>98</v>
       </c>
       <c r="D37" t="s">
         <v>101</v>
@@ -1395,7 +1401,7 @@
         <v>102</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D38" t="s">
         <v>103</v>
@@ -1409,10 +1415,10 @@
         <v>104</v>
       </c>
       <c r="C39" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" t="s">
         <v>105</v>
-      </c>
-      <c r="D39" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1420,13 +1426,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40" t="s">
         <v>107</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>108</v>
-      </c>
-      <c r="D40" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1434,10 +1440,10 @@
         <v>38</v>
       </c>
       <c r="B41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" t="s">
         <v>110</v>
-      </c>
-      <c r="C41" t="s">
-        <v>108</v>
       </c>
       <c r="D41" t="s">
         <v>111</v>
@@ -1451,7 +1457,7 @@
         <v>112</v>
       </c>
       <c r="C42" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D42" t="s">
         <v>113</v>
@@ -1465,7 +1471,7 @@
         <v>114</v>
       </c>
       <c r="C43" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D43" t="s">
         <v>115</v>
@@ -1479,7 +1485,7 @@
         <v>116</v>
       </c>
       <c r="C44" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D44" t="s">
         <v>117</v>
@@ -1493,7 +1499,7 @@
         <v>118</v>
       </c>
       <c r="C45" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D45" t="s">
         <v>119</v>
@@ -1507,7 +1513,7 @@
         <v>120</v>
       </c>
       <c r="C46" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D46" t="s">
         <v>121</v>
@@ -1521,7 +1527,7 @@
         <v>122</v>
       </c>
       <c r="C47" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D47" t="s">
         <v>123</v>
@@ -1535,7 +1541,7 @@
         <v>124</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D48" t="s">
         <v>125</v>
@@ -1549,7 +1555,7 @@
         <v>126</v>
       </c>
       <c r="C49" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D49" t="s">
         <v>127</v>
@@ -1563,7 +1569,7 @@
         <v>128</v>
       </c>
       <c r="C50" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D50" t="s">
         <v>129</v>
@@ -1577,7 +1583,7 @@
         <v>130</v>
       </c>
       <c r="C51" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D51" t="s">
         <v>131</v>
@@ -1591,7 +1597,7 @@
         <v>132</v>
       </c>
       <c r="C52" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D52" t="s">
         <v>133</v>
@@ -1605,7 +1611,7 @@
         <v>134</v>
       </c>
       <c r="C53" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D53" t="s">
         <v>135</v>
@@ -1619,7 +1625,7 @@
         <v>136</v>
       </c>
       <c r="C54" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D54" t="s">
         <v>137</v>
@@ -1633,7 +1639,7 @@
         <v>138</v>
       </c>
       <c r="C55" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="D55" t="s">
         <v>139</v>
@@ -1646,6 +1652,9 @@
       <c r="B56" t="s">
         <v>140</v>
       </c>
+      <c r="C56" t="s">
+        <v>110</v>
+      </c>
       <c r="D56" t="s">
         <v>141</v>
       </c>
@@ -1681,6 +1690,17 @@
       </c>
       <c r="D59" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" t="s">
+        <v>148</v>
+      </c>
+      <c r="D60" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update unit for Voltage-ampere-reactive
</commit_message>
<xml_diff>
--- a/import-specification/devices/battery.xlsx
+++ b/import-specification/devices/battery.xlsx
@@ -308,7 +308,7 @@
     <t>B_Q_AC</t>
   </si>
   <si>
-    <t>VAr</t>
+    <t>var</t>
   </si>
   <si>
     <t>Battery reactive power AC</t>
@@ -497,22 +497,23 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -811,7 +812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -823,14 +824,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="34.134521" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="56.557617" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="36.419678" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="34.135" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="8.141" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="56.558" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="12.854" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="36.42" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="11.569" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
@@ -1704,10 +1705,9 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>
@@ -1716,5 +1716,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New abbreviations for batteries
</commit_message>
<xml_diff>
--- a/import-specification/devices/battery.xlsx
+++ b/import-specification/devices/battery.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="169">
   <si>
     <t>Field Type</t>
   </si>
@@ -221,6 +221,12 @@
     <t>Currently stored energy</t>
   </si>
   <si>
+    <t>B_FCE_COUNT</t>
+  </si>
+  <si>
+    <t>FCE count (full cycle equivalent)</t>
+  </si>
+  <si>
     <t>B_F_AC</t>
   </si>
   <si>
@@ -230,6 +236,12 @@
     <t>Grid frequency</t>
   </si>
   <si>
+    <t>B_INV_COUNT</t>
+  </si>
+  <si>
+    <t>Number of connected inverters</t>
+  </si>
+  <si>
     <t>B_I_AC</t>
   </si>
   <si>
@@ -291,6 +303,12 @@
   </si>
   <si>
     <t>Discharge end voltage</t>
+  </si>
+  <si>
+    <t>B_LOGIC_BAT_COUNT</t>
+  </si>
+  <si>
+    <t>Number of connected logical batteries (combination of racks)</t>
   </si>
   <si>
     <t>B_OT_TOTAL</t>
@@ -855,7 +873,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -866,7 +884,7 @@
     <col min="1" max="1" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="34.135" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="8.141" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="58.843" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="71.84" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="36.42" bestFit="true" customWidth="true" style="0"/>
@@ -1253,11 +1271,8 @@
       <c r="B24" t="s">
         <v>68</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>69</v>
-      </c>
-      <c r="D24" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1265,13 +1280,13 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
         <v>71</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>72</v>
-      </c>
-      <c r="D25" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1279,13 +1294,10 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" t="s">
         <v>74</v>
-      </c>
-      <c r="C26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1293,10 +1305,10 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
         <v>76</v>
-      </c>
-      <c r="C27" t="s">
-        <v>72</v>
       </c>
       <c r="D27" t="s">
         <v>77</v>
@@ -1310,7 +1322,7 @@
         <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
         <v>79</v>
@@ -1324,7 +1336,7 @@
         <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
         <v>81</v>
@@ -1338,10 +1350,10 @@
         <v>82</v>
       </c>
       <c r="C30" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" t="s">
         <v>83</v>
-      </c>
-      <c r="D30" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1349,13 +1361,13 @@
         <v>38</v>
       </c>
       <c r="B31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" t="s">
         <v>85</v>
-      </c>
-      <c r="C31" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1363,13 +1375,13 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" t="s">
         <v>87</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>88</v>
-      </c>
-      <c r="D32" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1377,13 +1389,13 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" t="s">
         <v>90</v>
-      </c>
-      <c r="C33" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1391,13 +1403,13 @@
         <v>38</v>
       </c>
       <c r="B34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" t="s">
         <v>92</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>93</v>
-      </c>
-      <c r="D34" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1405,13 +1417,13 @@
         <v>38</v>
       </c>
       <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" t="s">
         <v>95</v>
-      </c>
-      <c r="C35" t="s">
-        <v>83</v>
-      </c>
-      <c r="D35" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1419,13 +1431,10 @@
         <v>38</v>
       </c>
       <c r="B36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" t="s">
         <v>97</v>
-      </c>
-      <c r="C36" t="s">
-        <v>83</v>
-      </c>
-      <c r="D36" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1433,13 +1442,13 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" t="s">
         <v>99</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>100</v>
-      </c>
-      <c r="D37" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1447,13 +1456,13 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" t="s">
         <v>102</v>
-      </c>
-      <c r="C38" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1461,13 +1470,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" t="s">
         <v>104</v>
-      </c>
-      <c r="C39" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1475,13 +1484,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" t="s">
         <v>107</v>
-      </c>
-      <c r="C40" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1489,13 +1498,13 @@
         <v>38</v>
       </c>
       <c r="B41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" t="s">
         <v>109</v>
-      </c>
-      <c r="C41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1503,10 +1512,10 @@
         <v>38</v>
       </c>
       <c r="B42" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" t="s">
         <v>111</v>
-      </c>
-      <c r="C42" t="s">
-        <v>43</v>
       </c>
       <c r="D42" t="s">
         <v>112</v>
@@ -1520,7 +1529,7 @@
         <v>113</v>
       </c>
       <c r="C43" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="D43" t="s">
         <v>114</v>
@@ -1548,10 +1557,10 @@
         <v>117</v>
       </c>
       <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" t="s">
         <v>118</v>
-      </c>
-      <c r="D45" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1559,13 +1568,13 @@
         <v>38</v>
       </c>
       <c r="B46" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" t="s">
         <v>120</v>
-      </c>
-      <c r="C46" t="s">
-        <v>121</v>
-      </c>
-      <c r="D46" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1573,13 +1582,13 @@
         <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C47" t="s">
-        <v>121</v>
+        <v>43</v>
       </c>
       <c r="D47" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1587,13 +1596,13 @@
         <v>38</v>
       </c>
       <c r="B48" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" t="s">
+        <v>124</v>
+      </c>
+      <c r="D48" t="s">
         <v>125</v>
-      </c>
-      <c r="C48" t="s">
-        <v>121</v>
-      </c>
-      <c r="D48" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1601,10 +1610,10 @@
         <v>38</v>
       </c>
       <c r="B49" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49" t="s">
         <v>127</v>
-      </c>
-      <c r="C49" t="s">
-        <v>121</v>
       </c>
       <c r="D49" t="s">
         <v>128</v>
@@ -1618,7 +1627,7 @@
         <v>129</v>
       </c>
       <c r="C50" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D50" t="s">
         <v>130</v>
@@ -1632,7 +1641,7 @@
         <v>131</v>
       </c>
       <c r="C51" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D51" t="s">
         <v>132</v>
@@ -1646,7 +1655,7 @@
         <v>133</v>
       </c>
       <c r="C52" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D52" t="s">
         <v>134</v>
@@ -1660,7 +1669,7 @@
         <v>135</v>
       </c>
       <c r="C53" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
       <c r="D53" t="s">
         <v>136</v>
@@ -1674,7 +1683,7 @@
         <v>137</v>
       </c>
       <c r="C54" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
       <c r="D54" t="s">
         <v>138</v>
@@ -1688,7 +1697,7 @@
         <v>139</v>
       </c>
       <c r="C55" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
       <c r="D55" t="s">
         <v>140</v>
@@ -1702,7 +1711,7 @@
         <v>141</v>
       </c>
       <c r="C56" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D56" t="s">
         <v>142</v>
@@ -1716,7 +1725,7 @@
         <v>143</v>
       </c>
       <c r="C57" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D57" t="s">
         <v>144</v>
@@ -1730,7 +1739,7 @@
         <v>145</v>
       </c>
       <c r="C58" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D58" t="s">
         <v>146</v>
@@ -1744,7 +1753,7 @@
         <v>147</v>
       </c>
       <c r="C59" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D59" t="s">
         <v>148</v>
@@ -1758,7 +1767,7 @@
         <v>149</v>
       </c>
       <c r="C60" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D60" t="s">
         <v>150</v>
@@ -1771,6 +1780,9 @@
       <c r="B61" t="s">
         <v>151</v>
       </c>
+      <c r="C61" t="s">
+        <v>92</v>
+      </c>
       <c r="D61" t="s">
         <v>152</v>
       </c>
@@ -1783,7 +1795,7 @@
         <v>153</v>
       </c>
       <c r="C62" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="D62" t="s">
         <v>154</v>
@@ -1796,6 +1808,9 @@
       <c r="B63" t="s">
         <v>155</v>
       </c>
+      <c r="C63" t="s">
+        <v>92</v>
+      </c>
       <c r="D63" t="s">
         <v>156</v>
       </c>
@@ -1818,6 +1833,9 @@
       <c r="B65" t="s">
         <v>159</v>
       </c>
+      <c r="C65" t="s">
+        <v>127</v>
+      </c>
       <c r="D65" t="s">
         <v>160</v>
       </c>
@@ -1831,6 +1849,39 @@
       </c>
       <c r="D66" t="s">
         <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67" t="s">
+        <v>163</v>
+      </c>
+      <c r="D67" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" t="s">
+        <v>165</v>
+      </c>
+      <c r="D68" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" t="s">
+        <v>38</v>
+      </c>
+      <c r="B69" t="s">
+        <v>167</v>
+      </c>
+      <c r="D69" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New abbreviations for meter
</commit_message>
<xml_diff>
--- a/import-specification/devices/battery.xlsx
+++ b/import-specification/devices/battery.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="163">
   <si>
     <t>Field Type</t>
   </si>
@@ -221,12 +221,6 @@
     <t>Currently stored energy</t>
   </si>
   <si>
-    <t>B_FCE_COUNT</t>
-  </si>
-  <si>
-    <t>FCE count (full cycle equivalent)</t>
-  </si>
-  <si>
     <t>B_F_AC</t>
   </si>
   <si>
@@ -236,12 +230,6 @@
     <t>Grid frequency</t>
   </si>
   <si>
-    <t>B_INV_COUNT</t>
-  </si>
-  <si>
-    <t>Number of connected inverters</t>
-  </si>
-  <si>
     <t>B_I_AC</t>
   </si>
   <si>
@@ -303,12 +291,6 @@
   </si>
   <si>
     <t>Discharge end voltage</t>
-  </si>
-  <si>
-    <t>B_LOGIC_BAT_COUNT</t>
-  </si>
-  <si>
-    <t>Number of connected logical batteries (combination of racks)</t>
   </si>
   <si>
     <t>B_OT_TOTAL</t>
@@ -873,7 +855,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -884,7 +866,7 @@
     <col min="1" max="1" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="34.135" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="8.141" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="71.84" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="58.843" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="36.42" bestFit="true" customWidth="true" style="0"/>
@@ -1271,8 +1253,11 @@
       <c r="B24" t="s">
         <v>68</v>
       </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1280,13 +1265,13 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1294,10 +1279,13 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1305,10 +1293,10 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
         <v>77</v>
@@ -1322,7 +1310,7 @@
         <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
         <v>79</v>
@@ -1336,7 +1324,7 @@
         <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D29" t="s">
         <v>81</v>
@@ -1350,10 +1338,10 @@
         <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1361,13 +1349,13 @@
         <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1375,13 +1363,13 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1389,13 +1377,13 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1403,13 +1391,13 @@
         <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C34" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D34" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1417,13 +1405,13 @@
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1431,10 +1419,13 @@
         <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+      <c r="C36" t="s">
+        <v>83</v>
       </c>
       <c r="D36" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1442,13 +1433,13 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D37" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1456,13 +1447,13 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D38" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1470,13 +1461,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C39" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="D39" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1484,13 +1475,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="D40" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1498,13 +1489,13 @@
         <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="D41" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1512,10 +1503,10 @@
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>43</v>
       </c>
       <c r="D42" t="s">
         <v>112</v>
@@ -1529,7 +1520,7 @@
         <v>113</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="D43" t="s">
         <v>114</v>
@@ -1557,10 +1548,10 @@
         <v>117</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="D45" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1568,13 +1559,13 @@
         <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C46" t="s">
-        <v>43</v>
+        <v>121</v>
       </c>
       <c r="D46" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1582,13 +1573,13 @@
         <v>38</v>
       </c>
       <c r="B47" t="s">
+        <v>123</v>
+      </c>
+      <c r="C47" t="s">
         <v>121</v>
       </c>
-      <c r="C47" t="s">
-        <v>43</v>
-      </c>
       <c r="D47" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1596,13 +1587,13 @@
         <v>38</v>
       </c>
       <c r="B48" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C48" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1610,10 +1601,10 @@
         <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C49" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D49" t="s">
         <v>128</v>
@@ -1627,7 +1618,7 @@
         <v>129</v>
       </c>
       <c r="C50" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D50" t="s">
         <v>130</v>
@@ -1641,7 +1632,7 @@
         <v>131</v>
       </c>
       <c r="C51" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D51" t="s">
         <v>132</v>
@@ -1655,7 +1646,7 @@
         <v>133</v>
       </c>
       <c r="C52" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D52" t="s">
         <v>134</v>
@@ -1669,7 +1660,7 @@
         <v>135</v>
       </c>
       <c r="C53" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="D53" t="s">
         <v>136</v>
@@ -1683,7 +1674,7 @@
         <v>137</v>
       </c>
       <c r="C54" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="D54" t="s">
         <v>138</v>
@@ -1697,7 +1688,7 @@
         <v>139</v>
       </c>
       <c r="C55" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="D55" t="s">
         <v>140</v>
@@ -1711,7 +1702,7 @@
         <v>141</v>
       </c>
       <c r="C56" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D56" t="s">
         <v>142</v>
@@ -1725,7 +1716,7 @@
         <v>143</v>
       </c>
       <c r="C57" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D57" t="s">
         <v>144</v>
@@ -1739,7 +1730,7 @@
         <v>145</v>
       </c>
       <c r="C58" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D58" t="s">
         <v>146</v>
@@ -1753,7 +1744,7 @@
         <v>147</v>
       </c>
       <c r="C59" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D59" t="s">
         <v>148</v>
@@ -1767,7 +1758,7 @@
         <v>149</v>
       </c>
       <c r="C60" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D60" t="s">
         <v>150</v>
@@ -1780,9 +1771,6 @@
       <c r="B61" t="s">
         <v>151</v>
       </c>
-      <c r="C61" t="s">
-        <v>92</v>
-      </c>
       <c r="D61" t="s">
         <v>152</v>
       </c>
@@ -1795,7 +1783,7 @@
         <v>153</v>
       </c>
       <c r="C62" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="D62" t="s">
         <v>154</v>
@@ -1808,9 +1796,6 @@
       <c r="B63" t="s">
         <v>155</v>
       </c>
-      <c r="C63" t="s">
-        <v>92</v>
-      </c>
       <c r="D63" t="s">
         <v>156</v>
       </c>
@@ -1833,9 +1818,6 @@
       <c r="B65" t="s">
         <v>159</v>
       </c>
-      <c r="C65" t="s">
-        <v>127</v>
-      </c>
       <c r="D65" t="s">
         <v>160</v>
       </c>
@@ -1849,39 +1831,6 @@
       </c>
       <c r="D66" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="A67" t="s">
-        <v>38</v>
-      </c>
-      <c r="B67" t="s">
-        <v>163</v>
-      </c>
-      <c r="D67" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
-      <c r="A68" t="s">
-        <v>38</v>
-      </c>
-      <c r="B68" t="s">
-        <v>165</v>
-      </c>
-      <c r="D68" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
-      <c r="A69" t="s">
-        <v>38</v>
-      </c>
-      <c r="B69" t="s">
-        <v>167</v>
-      </c>
-      <c r="D69" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>